<commit_message>
Adding to E2E tests.
</commit_message>
<xml_diff>
--- a/front-end/images/user-stories.xlsx
+++ b/front-end/images/user-stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kckar\Desktop\Revature\project1_reimbursements\front-end\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D7DDB3-C664-488A-B3FD-5674195AF108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B13A86-2AF0-4D5B-85AE-FE0C0790F159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{777FCCFE-CD23-40EF-8C42-5A7CABC9698D}"/>
   </bookViews>
@@ -81,24 +81,6 @@
     <t>I can view all reimbursements requested.</t>
   </si>
   <si>
-    <t>to approve reimbursement requests</t>
-  </si>
-  <si>
-    <t>to deny reimbursement requests</t>
-  </si>
-  <si>
-    <t>they are legitimate.</t>
-  </si>
-  <si>
-    <t>they are not legitimate.</t>
-  </si>
-  <si>
-    <t>to leave a comment about my decision</t>
-  </si>
-  <si>
-    <t>employees will understand my choices.</t>
-  </si>
-  <si>
     <t>to view reimbursement statistics</t>
   </si>
   <si>
@@ -136,6 +118,24 @@
   </si>
   <si>
     <t>Scenario: As an employee I want to log out so that my information will not remain on the computer.                           Given the employee is on the employee home page.             When the employee clicks on the log out button.                      Then they will be logged out.</t>
+  </si>
+  <si>
+    <t>Feature: using the manager home page in the reimbursement system.                                                                                        Scenario: As a manager I want to login so that I can view all the reimbursements requested.                                                          Given the manager is on the login page.                                    When the manager fills in id in the input space.                      When the manager fills in password in the input space.                                                                                               When the manager clicks the login button.                                Then they will be logged in.</t>
+  </si>
+  <si>
+    <t>to approve or deny reimbursement requests</t>
+  </si>
+  <si>
+    <t>if they are legitimate or not.</t>
+  </si>
+  <si>
+    <t>Scenario: As a manager I want to approve or deny reimbursement requests if they are legitimate or not.                                                    Given the manager is on the manager home page.                When the manager clicks on the submit reimbursement status tab.                                                                                                     When the manager fills out the reimbursement id.                When the manager selects approved or denied from the drop down options.                                                                                            When the manager fills out the reason input.                            When the manager clicks the submit status button.                 Then the status will be submitted.</t>
+  </si>
+  <si>
+    <t>Scenario: As a manager I want to view reimbursement statistics so that I can keep track of employee activities.                          Given the manager is on the manager home page.                  When the manager clicks the view reimbursement statistics tab.  When the manager selects the statistics option from the dropdown.                                                                                       When the manager clicks the statistics submit button.            Then the statistics are shown.</t>
+  </si>
+  <si>
+    <t>Scenario: As a manager I want to log out so that my information will not remain on the computer.                                                Given the manager is on the manager home page.                 When the manager clicks on the logout button.                        Then the manager is redirected to the login page.</t>
   </si>
 </sst>
 </file>
@@ -280,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -300,6 +300,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -616,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4DF1BB-8F48-4F24-8A0C-CAB16CA1BEF3}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,8 +660,8 @@
       <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>30</v>
+      <c r="F3" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -674,8 +677,8 @@
       <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>31</v>
+      <c r="F5" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -691,8 +694,8 @@
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>32</v>
+      <c r="F7" s="15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -708,8 +711,8 @@
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>33</v>
+      <c r="F9" s="15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -717,7 +720,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -727,79 +730,103 @@
       <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="F12" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="10"/>
+      <c r="B18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="9"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="9"/>
+      <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="4" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="9"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
-      <c r="B21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>28</v>
+      <c r="C25" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>